<commit_message>
Added a line for Table 2
</commit_message>
<xml_diff>
--- a/_readme/table-mapping.xlsx
+++ b/_readme/table-mapping.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sylverie/Dropbox/My Mac (sylveries-macbook-pro.home)/Desktop/aej-applied-replications-public/_readme/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lv39\Documents\GitHub\aej-applied-replications-public\_readme\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0952592-958B-4AB5-840F-406F3E17B40F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15000" yWindow="460" windowWidth="22600" windowHeight="16720" tabRatio="500"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15466" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table-mapping" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="133">
   <si>
     <t>Table number</t>
   </si>
@@ -423,12 +424,15 @@
   </si>
   <si>
     <t>A17</t>
+  </si>
+  <si>
+    <t>No code</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -467,6 +471,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -581,24 +588,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C62"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="86" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.46875" defaultRowHeight="12.7" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="44.33203125" customWidth="1"/>
+    <col min="1" max="2" width="44.3515625" customWidth="1"/>
     <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="7.5" customWidth="1"/>
-    <col min="5" max="5" width="3.1640625" customWidth="1"/>
+    <col min="4" max="4" width="7.46875" customWidth="1"/>
+    <col min="5" max="5" width="3.17578125" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.64453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -609,390 +616,390 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>2</v>
+      </c>
       <c r="B2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A5">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
         <v>127</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B7" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B8" t="s">
         <v>13</v>
-      </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A8">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A9" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
         <v>131</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>16</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A10">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A11">
         <v>16</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B11" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B12" t="s">
         <v>20</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C12" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B12" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B13" t="s">
         <v>22</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C13" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A13">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A14">
         <v>9</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>24</v>
-      </c>
-      <c r="C13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B14" t="s">
-        <v>26</v>
       </c>
       <c r="C14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B16" t="s">
         <v>27</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A16" t="s">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
         <v>129</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>29</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B17" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B18" t="s">
         <v>31</v>
-      </c>
-      <c r="C17" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A18" t="s">
-        <v>125</v>
-      </c>
-      <c r="B18" t="s">
-        <v>33</v>
       </c>
       <c r="C18" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
+        <v>125</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
         <v>119</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>34</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A20">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A21">
         <v>11</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>36</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C21" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A21" t="s">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
         <v>121</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>38</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A22" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
         <v>120</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>40</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A23" t="s">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
         <v>130</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>42</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A24" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
         <v>126</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>44</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B25" t="s">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B26" t="s">
         <v>46</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C26" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A26">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A27">
         <v>13</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>48</v>
-      </c>
-      <c r="C26" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B27" t="s">
-        <v>50</v>
       </c>
       <c r="C27" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A28">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B28" t="s">
+        <v>50</v>
+      </c>
+      <c r="C28" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A29">
         <v>10</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B29" t="s">
         <v>51</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C29" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B29" t="s">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B30" t="s">
         <v>53</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C30" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A30">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A31">
         <v>14</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B31" t="s">
         <v>55</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C31" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B31" t="s">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B32" t="s">
         <v>57</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C32" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B32" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B33" t="s">
         <v>59</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C33" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B33" t="s">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B34" t="s">
         <v>61</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C34" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A34" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A35" t="s">
         <v>128</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>63</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B35" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B36" t="s">
         <v>65</v>
-      </c>
-      <c r="C35" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A36" t="s">
-        <v>124</v>
-      </c>
-      <c r="B36" t="s">
-        <v>67</v>
       </c>
       <c r="C36" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A37" t="s">
+        <v>124</v>
+      </c>
+      <c r="B37" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A38" t="s">
         <v>118</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>68</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C38" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A38">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A39">
         <v>12</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>70</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C39" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B39" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B40" t="s">
         <v>72</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B40" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B41" t="s">
         <v>74</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B41" t="s">
-        <v>76</v>
-      </c>
-      <c r="C41" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B42" t="s">
         <v>76</v>
       </c>
@@ -1000,7 +1007,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.4">
       <c r="B43" t="s">
         <v>76</v>
       </c>
@@ -1008,191 +1015,199 @@
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A44" t="s">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B44" t="s">
+        <v>76</v>
+      </c>
+      <c r="C44" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A45" t="s">
         <v>122</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>78</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A45" t="s">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A46" t="s">
         <v>123</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>80</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B46" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B47" t="s">
         <v>82</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C47" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A47" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A48" t="s">
         <v>116</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>84</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C48" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A48">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A49">
         <v>1</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>86</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A49" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A50" t="s">
         <v>115</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>88</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C50" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A50">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A51">
         <v>3</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>90</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A51">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A52">
         <v>4</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>92</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C52" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B52" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B53" t="s">
         <v>94</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C53" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B53" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B54" t="s">
         <v>96</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C54" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A54">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A55">
         <v>5</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B55" t="s">
         <v>98</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C55" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B55" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B56" t="s">
         <v>100</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C56" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A56">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A57">
         <v>6</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>102</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C57" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B57" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B58" t="s">
         <v>104</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C58" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A58">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A59">
         <v>8</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B59" t="s">
         <v>106</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C59" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B59" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B60" t="s">
         <v>108</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C60" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A60">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A61">
         <v>7</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>110</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C61" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A61" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A62" t="s">
         <v>117</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>112</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C62" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="B62" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="B63" t="s">
         <v>114</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C63" t="s">
         <v>111</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adjusting one table mapping
</commit_message>
<xml_diff>
--- a/_readme/table-mapping.xlsx
+++ b/_readme/table-mapping.xlsx
@@ -496,8 +496,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -627,622 +631,622 @@
   <dimension ref="A1:C63"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="86" zoomScaleNormal="86" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
+      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.47265625" defaultRowHeight="12" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="44.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="7.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="3.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="11.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="44.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="3.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.65"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
+      <c r="A9" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
+      <c r="A11" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
+      <c r="A14" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="0" t="s">
+      <c r="B17" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="0" t="s">
+      <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="0" t="s">
+      <c r="B19" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
+      <c r="A21" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B21" s="0" t="s">
+      <c r="B21" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="0" t="s">
+      <c r="B22" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B23" s="0" t="s">
+      <c r="B23" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="0" t="s">
+      <c r="B24" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="0" t="s">
+      <c r="B25" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="0" t="s">
+      <c r="B26" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B27" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" s="0" t="s">
+      <c r="B28" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="C28" s="0" t="s">
-        <v>60</v>
-      </c>
-    </row>
     <row r="29" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="n">
+      <c r="A29" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B29" s="0" t="s">
+      <c r="B29" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="0" t="s">
+      <c r="B30" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
+      <c r="A31" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B31" s="0" t="s">
+      <c r="B31" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="0" t="s">
+      <c r="B32" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="0" t="s">
+      <c r="B33" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="0" t="s">
+      <c r="B34" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="C34" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="C35" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B37" s="0" t="s">
+      <c r="B37" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C37" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B38" s="0" t="s">
+      <c r="B38" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C38" s="0" t="s">
+      <c r="C38" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="n">
+      <c r="A39" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B39" s="0" t="s">
+      <c r="B39" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C39" s="0" t="s">
+      <c r="C39" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="0" t="s">
+      <c r="B40" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C40" s="0" t="s">
+      <c r="C40" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="0" t="s">
+      <c r="B41" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="C41" s="1" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="0" t="s">
+      <c r="B42" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C42" s="0" t="s">
+      <c r="C42" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="0" t="s">
+      <c r="B43" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="C43" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="0" t="s">
+      <c r="B44" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C44" s="0" t="s">
+      <c r="C44" s="1" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="B45" s="0" t="s">
+      <c r="B45" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="C45" s="1" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="B46" s="0" t="s">
+      <c r="B46" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="C46" s="1" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="0" t="s">
+      <c r="B47" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C47" s="0" t="s">
+      <c r="C47" s="1" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="B48" s="0" t="s">
+      <c r="B48" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="C48" s="0" t="s">
+      <c r="C48" s="1" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="n">
+      <c r="A49" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B49" s="0" t="s">
+      <c r="B49" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C49" s="0" t="s">
+      <c r="C49" s="1" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B50" s="0" t="s">
+      <c r="B50" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C50" s="0" t="s">
+      <c r="C50" s="1" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="n">
+      <c r="A51" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B51" s="0" t="s">
+      <c r="B51" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C51" s="0" t="s">
+      <c r="C51" s="1" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="n">
+      <c r="A52" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B52" s="0" t="s">
+      <c r="B52" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="C52" s="0" t="s">
+      <c r="C52" s="1" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="0" t="s">
+      <c r="B53" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C53" s="0" t="s">
+      <c r="C53" s="1" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="0" t="s">
+      <c r="B54" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C54" s="0" t="s">
+      <c r="C54" s="1" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="n">
+      <c r="A55" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B55" s="0" t="s">
+      <c r="B55" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C55" s="0" t="s">
+      <c r="C55" s="1" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="0" t="s">
+      <c r="B56" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="C56" s="0" t="s">
+      <c r="C56" s="1" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="n">
+      <c r="A57" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B57" s="0" t="s">
+      <c r="B57" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C57" s="0" t="s">
+      <c r="C57" s="1" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="0" t="s">
+      <c r="B58" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C58" s="0" t="s">
+      <c r="C58" s="1" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="n">
+      <c r="A59" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B59" s="0" t="s">
+      <c r="B59" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C59" s="0" t="s">
+      <c r="C59" s="1" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="0" t="s">
+      <c r="B60" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C60" s="0" t="s">
+      <c r="C60" s="1" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="n">
+      <c r="A61" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B61" s="0" t="s">
+      <c r="B61" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C61" s="0" t="s">
+      <c r="C61" s="1" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+      <c r="A62" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B62" s="0" t="s">
+      <c r="B62" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="C62" s="0" t="s">
+      <c r="C62" s="1" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="0" t="s">
+      <c r="B63" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C63" s="0" t="s">
+      <c r="C63" s="1" t="s">
         <v>129</v>
       </c>
     </row>

</xml_diff>